<commit_message>
Matriz actualizada al 2026
Se añadió el primer atentado 2026
</commit_message>
<xml_diff>
--- a/docs/RMD2_Matriz_Araucania.xlsx
+++ b/docs/RMD2_Matriz_Araucania.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X318"/>
+  <dimension ref="A1:X319"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -31509,6 +31509,76 @@
         <v>33.33333333333333</v>
       </c>
     </row>
+    <row r="319">
+      <c r="A319" t="n">
+        <v>318</v>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Atentado incendiario: queman 2 máquinas excavadoras en sector La Junta</t>
+        </is>
+      </c>
+      <c r="C319" t="n">
+        <v>46024</v>
+      </c>
+      <c r="D319" t="n">
+        <v>46024</v>
+      </c>
+      <c r="E319" t="inlineStr">
+        <is>
+          <t>Nueva Imperial</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
+          <t>Ataque incendiario</t>
+        </is>
+      </c>
+      <c r="G319" t="inlineStr"/>
+      <c r="H319" t="inlineStr"/>
+      <c r="I319" t="inlineStr"/>
+      <c r="J319" t="inlineStr"/>
+      <c r="K319" t="inlineStr">
+        <is>
+          <t>Atentado incendiario en parcela destinada al acopio de áridos en el sector rural La Junta. Dos máquinas excavadoras resultaron destruidas (separadas aprox. 500 m). Fiscalía instruyó diligencias a BIPE y Laboratorio de Criminalística PDI; sin lienzos ni mensajes de atribución.</t>
+        </is>
+      </c>
+      <c r="L319" t="inlineStr">
+        <is>
+          <t>Actualización 2026 (OSINT triangulado).</t>
+        </is>
+      </c>
+      <c r="M319" t="inlineStr">
+        <is>
+          <t>Acoforag (02/01/2026) https://www.acoforag.cl/es/noticias/2026/1/2/primer-atentado-del-ano-en-la-araucania-deja-dos-maquinas-destruidas/ | Emol (02/01/2026) https://www.emol.com/noticias/Nacional/2026/01/02/1187436/atentado-incendiario--la-araucania.html | AraucaniaDiario (03/01/2026) https://araucaniadiario.cl/contenido/31745/con-un-atentado-en-imperial-parte-el-ano-la-violencia-rural-en-la-araucania | ADN Radio (02/01/2026) https://www.adnradio.cl/2026/01/02/reportan-el-primer-atentado-incendiario-del-ano-en-la-araucania-dos-excavadoras-destruidas-en-nueva-imperial/</t>
+        </is>
+      </c>
+      <c r="N319" t="inlineStr"/>
+      <c r="O319" t="inlineStr"/>
+      <c r="P319" t="inlineStr">
+        <is>
+          <t>Araucanía</t>
+        </is>
+      </c>
+      <c r="Q319" t="inlineStr"/>
+      <c r="R319" t="inlineStr"/>
+      <c r="S319" s="2" t="n">
+        <v>46024</v>
+      </c>
+      <c r="T319" t="n">
+        <v>2026</v>
+      </c>
+      <c r="U319" t="n">
+        <v>1</v>
+      </c>
+      <c r="V319" t="inlineStr">
+        <is>
+          <t>2026-01</t>
+        </is>
+      </c>
+      <c r="W319" t="inlineStr"/>
+      <c r="X319" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>